<commit_message>
Add COG Dataset 6 to pipeline
</commit_message>
<xml_diff>
--- a/MetricList.xlsx
+++ b/MetricList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kobifeldman\Code-Complexity-Research\complexity-verification-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C52F87-FE8E-4F8C-AB15-FA6968AD867B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5626AC50-2B40-42C7-B810-DD442D1591CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
   </bookViews>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update MetricList.xlsx for consistency with cog study
</commit_message>
<xml_diff>
--- a/MetricList.xlsx
+++ b/MetricList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kobifeldman\Code-Complexity-Research\complexity-verification-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E95046-5C3F-48B8-9AD1-05FAAF644B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E272D8A4-0338-4BAD-BA43-7703E9181B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>Dataset</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>Metric Explanation</t>
-  </si>
-  <si>
     <t>COG Dataset 1</t>
   </si>
   <si>
@@ -78,15 +75,6 @@
     <t>percieved_readability</t>
   </si>
   <si>
-    <t>time for participant to understand snippet in seconds, not limited</t>
-  </si>
-  <si>
-    <t>0 = completely wrong, 1 = partialy correct, 2 = completely correct</t>
-  </si>
-  <si>
-    <t>scale of 1 to 5, 1 = less readable, 5 = more readable</t>
-  </si>
-  <si>
     <t>time for participant to understand snippet in seconds, limited to 60 sec.</t>
   </si>
   <si>
@@ -114,18 +102,6 @@
     <t>pbu (Perceived Binary Understandability)</t>
   </si>
   <si>
-    <t>time in seconds spent by the participant on trying to understand a snippet</t>
-  </si>
-  <si>
-    <t>percentage of correct answers given by the participants to 3 verification questions</t>
-  </si>
-  <si>
-    <t>true = participant clicked button saying they understood, false = participant clicked button saying they couldn't understand the snippet</t>
-  </si>
-  <si>
-    <t>scale of 0 through 4 where 0 = very difficult, 1 = difficult, 2 = medium, 3 = easy, 4 = very easy</t>
-  </si>
-  <si>
     <t>https://arxiv.org/abs/2007.12520, https://ieeexplore-ieee-org.proxy.wm.edu/stamp/stamp.jsp?tp=&amp;arnumber=8425769</t>
   </si>
   <si>
@@ -159,9 +135,6 @@
     <t>BA31ant</t>
   </si>
   <si>
-    <t>time values in the hundred thousands values so probabably something like 600000 = 60000.0 ms = 60 s since there is a 60 second limit</t>
-  </si>
-  <si>
     <t>https://arxiv.org/abs/2007.12520, https://ieeexplore-ieee-org.proxy.wm.edu/stamp/stamp.jsp?tp=&amp;arnumber=8425770</t>
   </si>
   <si>
@@ -175,9 +148,6 @@
   </si>
   <si>
     <t>COG Dataset 9</t>
-  </si>
-  <si>
-    <t>pooled_time</t>
   </si>
   <si>
     <t>acc</t>
@@ -209,6 +179,66 @@
   </si>
   <si>
     <t>Longer explanations are in "Dataset Decisions" Google Doc in the shared Drive</t>
+  </si>
+  <si>
+    <t>Time taken in seconds to understand the code and answer one question. (Calculate output)</t>
+  </si>
+  <si>
+    <t>Metric explanations taken from reading/understanding the associated paper + using the cog complexity study metric descriptions which can be found in dataset.xlsx in the analysis package cited as the 3rd source on their paper.</t>
+  </si>
+  <si>
+    <t>Metric Description</t>
+  </si>
+  <si>
+    <t>0: completely wrong, 1: in part correct, 2: completely correct (Calculate output)</t>
+  </si>
+  <si>
+    <t>0: very difficult, 1: difficult, 2: medium, 3: easy, 4: very easy (How difficult did you think determining the output of the method was?)</t>
+  </si>
+  <si>
+    <t>Time taken in seconds until the participant indicated they understood the code. Limited to max 60 seconds.</t>
+  </si>
+  <si>
+    <t>average strength of brain deactivation</t>
+  </si>
+  <si>
+    <t>From 1 less readable to 5 more readable. Participants score each snippet based on their personal estimation of readability. When users clicked help, they were reminded that “readability is their judgment about how easy a block of code is to understand.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time taken in seconds until the participant indicated they understood the code. </t>
+  </si>
+  <si>
+    <t>Percentage of correct answers to the three verification questions. If the participant said they did not understand the snippet earlier, the value is 0.</t>
+  </si>
+  <si>
+    <t>1 if the participant said they understood the snippet, 0 if not.</t>
+  </si>
+  <si>
+    <t>Time taken in seconds until the participant submitted their readability rating.</t>
+  </si>
+  <si>
+    <t>Time taken in seconds to complete the cloze task.</t>
+  </si>
+  <si>
+    <t>Recall accuracy of the participant in the cloze test.</t>
+  </si>
+  <si>
+    <t>From 1 less readable to 5 more readable. Initial readability rating after reading the snippet.</t>
+  </si>
+  <si>
+    <t>From 1 less readable to 5 more readable. Readability rating after the cloze test.</t>
+  </si>
+  <si>
+    <t>pooled_rating - r1</t>
+  </si>
+  <si>
+    <t>pooled_rating - r2</t>
+  </si>
+  <si>
+    <t>pooled_time - tr</t>
+  </si>
+  <si>
+    <t>pooled_time - ta</t>
   </si>
 </sst>
 </file>
@@ -620,18 +650,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="93.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
   </cols>
@@ -644,10 +674,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -655,269 +685,326 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
       <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
-        <v>50</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -927,9 +1014,9 @@
     <hyperlink ref="E3" r:id="rId2" display="https://arxiv.org/abs/2007.12520" xr:uid="{66AD7CC2-BE01-4EC0-BAE7-28EDE782EFDA}"/>
     <hyperlink ref="E4" r:id="rId3" display="https://arxiv.org/abs/2007.12520" xr:uid="{A0BEBDA8-27CE-4A6A-94E5-567D3B368EE4}"/>
     <hyperlink ref="E9" r:id="rId4" display="https://arxiv.org/abs/2007.12520" xr:uid="{60B3F41B-30C2-43E1-B421-E4D90470F87D}"/>
-    <hyperlink ref="E16" r:id="rId5" xr:uid="{499C2C3A-FABB-45A5-AE79-5D4E6E7909CC}"/>
-    <hyperlink ref="E17" r:id="rId6" xr:uid="{DA11740A-18E4-4E87-BDAD-5E5F66D65697}"/>
-    <hyperlink ref="E18" r:id="rId7" xr:uid="{1E3786EB-DE0D-4C58-A525-CFD47EC052FA}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{499C2C3A-FABB-45A5-AE79-5D4E6E7909CC}"/>
+    <hyperlink ref="E19" r:id="rId6" xr:uid="{DA11740A-18E4-4E87-BDAD-5E5F66D65697}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{1E3786EB-DE0D-4C58-A525-CFD47EC052FA}"/>
     <hyperlink ref="E10:E12" r:id="rId8" display="https://arxiv.org/abs/2007.12520" xr:uid="{A7160B9F-EEB9-4C4D-BEBE-7200AA34C448}"/>
     <hyperlink ref="E5:E8" r:id="rId9" display="https://arxiv.org/abs/2007.12520" xr:uid="{F4FEFDF7-D171-45D9-8872-FDBC183E038D}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
correlation results tables: rename of metrics and column changes
</commit_message>
<xml_diff>
--- a/MetricList.xlsx
+++ b/MetricList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kobifeldman\Code-Complexity-Research\complexity-verification-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E272D8A4-0338-4BAD-BA43-7703E9181B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651E1745-B0DC-2646-ACC6-863856B0B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
+    <workbookView xWindow="-120" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,29 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
-  <si>
-    <t>Dataset</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Metric</t>
-  </si>
-  <si>
     <t>COG Dataset 1</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Correctness</t>
-  </si>
-  <si>
-    <t>Rating</t>
-  </si>
-  <si>
     <t>COG Dataset 3</t>
   </si>
   <si>
@@ -90,9 +75,6 @@
     <t>COG Dataset 6</t>
   </si>
   <si>
-    <t>Metric Name in COG Paper</t>
-  </si>
-  <si>
     <t>tnpu (Time Needed for Percieved Understandability)</t>
   </si>
   <si>
@@ -118,9 +100,6 @@
   </si>
   <si>
     <t>COG Dataset 2</t>
-  </si>
-  <si>
-    <t>Physiological</t>
   </si>
   <si>
     <t>response_time</t>
@@ -187,9 +166,6 @@
     <t>Metric explanations taken from reading/understanding the associated paper + using the cog complexity study metric descriptions which can be found in dataset.xlsx in the analysis package cited as the 3rd source on their paper.</t>
   </si>
   <si>
-    <t>Metric Description</t>
-  </si>
-  <si>
     <t>0: completely wrong, 1: in part correct, 2: completely correct (Calculate output)</t>
   </si>
   <si>
@@ -239,13 +215,40 @@
   </si>
   <si>
     <t>pooled_time - ta</t>
+  </si>
+  <si>
+    <t>correctness</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>physiological</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>dataset_name</t>
+  </si>
+  <si>
+    <t>dataset_id</t>
+  </si>
+  <si>
+    <t>metric_type</t>
+  </si>
+  <si>
+    <t>metric_cog_paper</t>
+  </si>
+  <si>
+    <t>metric_decription</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +299,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -327,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -335,6 +345,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -650,375 +669,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="93.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="7">
+        <v>9</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E22" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="4" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://arxiv.org/abs/2007.12520" xr:uid="{514C6F19-B34F-4BE4-9C2B-92A41DC40E10}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://arxiv.org/abs/2007.12520" xr:uid="{66AD7CC2-BE01-4EC0-BAE7-28EDE782EFDA}"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://arxiv.org/abs/2007.12520" xr:uid="{A0BEBDA8-27CE-4A6A-94E5-567D3B368EE4}"/>
-    <hyperlink ref="E9" r:id="rId4" display="https://arxiv.org/abs/2007.12520" xr:uid="{60B3F41B-30C2-43E1-B421-E4D90470F87D}"/>
-    <hyperlink ref="E18" r:id="rId5" xr:uid="{499C2C3A-FABB-45A5-AE79-5D4E6E7909CC}"/>
-    <hyperlink ref="E19" r:id="rId6" xr:uid="{DA11740A-18E4-4E87-BDAD-5E5F66D65697}"/>
-    <hyperlink ref="E20" r:id="rId7" xr:uid="{1E3786EB-DE0D-4C58-A525-CFD47EC052FA}"/>
-    <hyperlink ref="E10:E12" r:id="rId8" display="https://arxiv.org/abs/2007.12520" xr:uid="{A7160B9F-EEB9-4C4D-BEBE-7200AA34C448}"/>
-    <hyperlink ref="E5:E8" r:id="rId9" display="https://arxiv.org/abs/2007.12520" xr:uid="{F4FEFDF7-D171-45D9-8872-FDBC183E038D}"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://arxiv.org/abs/2007.12520" xr:uid="{514C6F19-B34F-4BE4-9C2B-92A41DC40E10}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://arxiv.org/abs/2007.12520" xr:uid="{66AD7CC2-BE01-4EC0-BAE7-28EDE782EFDA}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://arxiv.org/abs/2007.12520" xr:uid="{A0BEBDA8-27CE-4A6A-94E5-567D3B368EE4}"/>
+    <hyperlink ref="F9" r:id="rId4" display="https://arxiv.org/abs/2007.12520" xr:uid="{60B3F41B-30C2-43E1-B421-E4D90470F87D}"/>
+    <hyperlink ref="F18" r:id="rId5" xr:uid="{499C2C3A-FABB-45A5-AE79-5D4E6E7909CC}"/>
+    <hyperlink ref="F19" r:id="rId6" xr:uid="{DA11740A-18E4-4E87-BDAD-5E5F66D65697}"/>
+    <hyperlink ref="F20" r:id="rId7" xr:uid="{1E3786EB-DE0D-4C58-A525-CFD47EC052FA}"/>
+    <hyperlink ref="F10:F12" r:id="rId8" display="https://arxiv.org/abs/2007.12520" xr:uid="{A7160B9F-EEB9-4C4D-BEBE-7200AA34C448}"/>
+    <hyperlink ref="F5:F8" r:id="rId9" display="https://arxiv.org/abs/2007.12520" xr:uid="{F4FEFDF7-D171-45D9-8872-FDBC183E038D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>

<commit_message>
update of forest plots based on new table columns
</commit_message>
<xml_diff>
--- a/MetricList.xlsx
+++ b/MetricList.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651E1745-B0DC-2646-ACC6-863856B0B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292EB398-4636-3D43-A360-733CE1941B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>Link</t>
   </si>
@@ -242,6 +245,60 @@
   </si>
   <si>
     <t>metric_decription</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>correct_output_rating</t>
+  </si>
+  <si>
+    <t>output_difficulty</t>
+  </si>
+  <si>
+    <t>time_to_give_output</t>
+  </si>
+  <si>
+    <t>brain_act_31ant</t>
+  </si>
+  <si>
+    <t>brain_act_31post</t>
+  </si>
+  <si>
+    <t>brain_act_32</t>
+  </si>
+  <si>
+    <t>time_to_understand</t>
+  </si>
+  <si>
+    <t>readability_level</t>
+  </si>
+  <si>
+    <t>correct_verif_questions</t>
+  </si>
+  <si>
+    <t>binary_understandability</t>
+  </si>
+  <si>
+    <t>gap_accuracy</t>
+  </si>
+  <si>
+    <t>readability_level_before</t>
+  </si>
+  <si>
+    <t>perc_correct_output</t>
+  </si>
+  <si>
+    <t>complexity_level</t>
+  </si>
+  <si>
+    <t>readability_level_after</t>
+  </si>
+  <si>
+    <t>time_to_read</t>
+  </si>
+  <si>
+    <t>time_to_complete</t>
   </si>
 </sst>
 </file>
@@ -315,7 +372,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -332,12 +389,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -353,6 +425,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -669,11 +744,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -681,12 +754,13 @@
     <col min="2" max="2" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93.6640625" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -699,14 +773,17 @@
       <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -714,19 +791,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -734,19 +814,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -754,19 +837,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -774,19 +860,22 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -797,16 +886,19 @@
         <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -817,16 +909,19 @@
         <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -834,19 +929,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -860,13 +958,16 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -874,19 +975,22 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -894,19 +998,22 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -914,19 +1021,22 @@
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -934,19 +1044,22 @@
         <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -954,19 +1067,22 @@
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -974,19 +1090,22 @@
         <v>9</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -994,19 +1113,22 @@
         <v>9</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1014,19 +1136,22 @@
         <v>9</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1034,16 +1159,19 @@
         <v>56</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1051,16 +1179,19 @@
         <v>56</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1068,37 +1199,45 @@
         <v>56</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E22" s="4" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F22" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E23" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F23" s="4" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G20" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+      <sortCondition ref="B1:B20"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://arxiv.org/abs/2007.12520" xr:uid="{514C6F19-B34F-4BE4-9C2B-92A41DC40E10}"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://arxiv.org/abs/2007.12520" xr:uid="{66AD7CC2-BE01-4EC0-BAE7-28EDE782EFDA}"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://arxiv.org/abs/2007.12520" xr:uid="{A0BEBDA8-27CE-4A6A-94E5-567D3B368EE4}"/>
-    <hyperlink ref="F9" r:id="rId4" display="https://arxiv.org/abs/2007.12520" xr:uid="{60B3F41B-30C2-43E1-B421-E4D90470F87D}"/>
-    <hyperlink ref="F18" r:id="rId5" xr:uid="{499C2C3A-FABB-45A5-AE79-5D4E6E7909CC}"/>
-    <hyperlink ref="F19" r:id="rId6" xr:uid="{DA11740A-18E4-4E87-BDAD-5E5F66D65697}"/>
-    <hyperlink ref="F20" r:id="rId7" xr:uid="{1E3786EB-DE0D-4C58-A525-CFD47EC052FA}"/>
-    <hyperlink ref="F10:F12" r:id="rId8" display="https://arxiv.org/abs/2007.12520" xr:uid="{A7160B9F-EEB9-4C4D-BEBE-7200AA34C448}"/>
-    <hyperlink ref="F5:F8" r:id="rId9" display="https://arxiv.org/abs/2007.12520" xr:uid="{F4FEFDF7-D171-45D9-8872-FDBC183E038D}"/>
+    <hyperlink ref="G4" r:id="rId1" display="https://arxiv.org/abs/2007.12520" xr:uid="{514C6F19-B34F-4BE4-9C2B-92A41DC40E10}"/>
+    <hyperlink ref="G2" r:id="rId2" display="https://arxiv.org/abs/2007.12520" xr:uid="{66AD7CC2-BE01-4EC0-BAE7-28EDE782EFDA}"/>
+    <hyperlink ref="G3" r:id="rId3" display="https://arxiv.org/abs/2007.12520" xr:uid="{A0BEBDA8-27CE-4A6A-94E5-567D3B368EE4}"/>
+    <hyperlink ref="G9" r:id="rId4" display="https://arxiv.org/abs/2007.12520" xr:uid="{60B3F41B-30C2-43E1-B421-E4D90470F87D}"/>
+    <hyperlink ref="G20" r:id="rId5" xr:uid="{499C2C3A-FABB-45A5-AE79-5D4E6E7909CC}"/>
+    <hyperlink ref="G18" r:id="rId6" xr:uid="{DA11740A-18E4-4E87-BDAD-5E5F66D65697}"/>
+    <hyperlink ref="G19" r:id="rId7" xr:uid="{1E3786EB-DE0D-4C58-A525-CFD47EC052FA}"/>
+    <hyperlink ref="G10:G12" r:id="rId8" display="https://arxiv.org/abs/2007.12520" xr:uid="{A7160B9F-EEB9-4C4D-BEBE-7200AA34C448}"/>
+    <hyperlink ref="G5:G8" r:id="rId9" display="https://arxiv.org/abs/2007.12520" xr:uid="{F4FEFDF7-D171-45D9-8872-FDBC183E038D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>

<commit_message>
Remove meta data from excel sheets
</commit_message>
<xml_diff>
--- a/MetricList.xlsx
+++ b/MetricList.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292EB398-4636-3D43-A360-733CE1941B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0C340D-2C35-4B5F-887B-AA75BA410F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -746,21 +741,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.6640625" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.7109375" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -783,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -806,7 +803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -829,7 +826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -852,7 +849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -875,7 +872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -898,7 +895,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -921,7 +918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -944,7 +941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -967,7 +964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -990,7 +987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1013,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1036,7 +1033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1082,7 +1079,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1128,7 +1125,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1151,7 +1148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1191,7 +1188,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1211,12 +1208,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F22" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F23" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
fixes related to measurements statistics
</commit_message>
<xml_diff>
--- a/MetricList.xlsx
+++ b/MetricList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292EB398-4636-3D43-A360-733CE1941B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13752CD7-F422-6E4C-848A-A4FE20649334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
+    <workbookView xWindow="-120" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{9D8E2941-33A1-42F9-8DF7-3DCAC8E8D453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>COG Dataset 6</t>
   </si>
   <si>
-    <t>tnpu (Time Needed for Percieved Understandability)</t>
-  </si>
-  <si>
     <t>au (Actual Understanding)</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>time_to_complete</t>
+  </si>
+  <si>
+    <t>tnpu (Time Needed for Perceived Understandability)</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DC268-181B-4678-9532-C1992D2903D0}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -762,22 +764,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -791,19 +793,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -814,19 +816,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -843,87 +845,87 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7">
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7">
         <v>2</v>
@@ -932,16 +934,16 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -952,19 +954,19 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -975,19 +977,19 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -998,19 +1000,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1024,90 +1026,90 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7">
         <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="7">
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="7">
         <v>9</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7">
         <v>9</v>
@@ -1116,21 +1118,21 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7">
         <v>9</v>
@@ -1139,16 +1141,16 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1156,13 +1158,13 @@
         <v>3</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -1176,13 +1178,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -1196,13 +1198,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -1213,12 +1215,12 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>